<commit_message>
channel column in write module added
</commit_message>
<xml_diff>
--- a/optimizer_windows/results.xlsx
+++ b/optimizer_windows/results.xlsx
@@ -14,12 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Channel</t>
+  </si>
   <si>
     <t>N</t>
   </si>
   <si>
     <t>Inversión</t>
+  </si>
+  <si>
+    <t>Televisión</t>
+  </si>
+  <si>
+    <t>Digital Video</t>
+  </si>
+  <si>
+    <t>Cine</t>
+  </si>
+  <si>
+    <t>BVOD</t>
   </si>
   <si>
     <t>Número de combinaciones</t>
@@ -357,13 +372,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,45 +389,60 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>543750</v>
+      </c>
+      <c r="D2">
+        <v>1216864</v>
+      </c>
+      <c r="E2">
+        <v>0.8605847883429888</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>540000</v>
-      </c>
-      <c r="C2">
-        <v>176850</v>
-      </c>
-      <c r="D2">
-        <v>0.8605609614996592</v>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>425000</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>420000</v>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>225000</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>228000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>12000</v>
+      <c r="C5">
+        <v>6250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>